<commit_message>
Updated to reflect sprint progress for monday
</commit_message>
<xml_diff>
--- a/Sprint2/SprintBacklog/Sprint 2 Backlog.xlsx
+++ b/Sprint2/SprintBacklog/Sprint 2 Backlog.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Submit Later\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Sprint 2</t>
   </si>
@@ -74,39 +82,47 @@
   </si>
   <si>
     <t>Just Started This Sprint</t>
+  </si>
+  <si>
+    <t>Successfully Completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -156,43 +172,62 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -202,94 +237,90 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -479,296 +510,324 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="30.0"/>
-    <col customWidth="1" min="16" max="16" width="30.29"/>
-    <col customWidth="1" min="17" max="17" width="27.14"/>
-    <col customWidth="1" min="18" max="18" width="22.0"/>
-    <col customWidth="1" min="19" max="19" width="20.71"/>
-    <col customWidth="1" min="23" max="23" width="21.71"/>
-    <col customWidth="1" min="24" max="24" width="33.71"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" customWidth="1"/>
+    <col min="17" max="17" width="27.140625" customWidth="1"/>
+    <col min="18" max="18" width="22" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" customWidth="1"/>
+    <col min="24" max="24" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="J2" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K2" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="L2" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M2" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="O2" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="P2" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="R2" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="S2" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="T2" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="U2" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="V2" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W2" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="X2" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="Y2" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="Z2" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="AA2" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="AB2" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="AC2" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="AD2" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="AE2" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="AF2" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="9" t="s">
+      <c r="R3" s="17"/>
+      <c r="S3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="11" t="s">
+      <c r="U3" s="16"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Y3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="6"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="17"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Y4" s="13" t="s">
         <v>14</v>
       </c>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
     </row>
-    <row r="5">
+    <row r="5" spans="2:32" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
     </row>
-    <row r="6">
+    <row r="6" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="18" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="23"/>
+      <c r="S6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="16"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="18" t="s">
+      <c r="Y6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="X6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="6"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="17"/>
     </row>
-    <row r="11">
-      <c r="B11" s="20"/>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
     </row>
-    <row r="12">
-      <c r="W12" s="21"/>
+    <row r="12" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W12" s="12"/>
     </row>
-    <row r="13">
-      <c r="M13" s="21"/>
+    <row r="13" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="C6:O6"/>
+    <mergeCell ref="C4:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:W4"/>
     <mergeCell ref="Y3:AD3"/>
     <mergeCell ref="Y4:AD4"/>
     <mergeCell ref="Y6:AD6"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="C6:O6"/>
-    <mergeCell ref="C4:P4"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="T6:V6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>